<commit_message>
Building SSIS & Adding Ref Data
Updating the SSIS package and amending the reference data where required to fit the model.
</commit_message>
<xml_diff>
--- a/referenceData/CircuitTypes.xlsx
+++ b/referenceData/CircuitTypes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\FormulaOneDatabase\referenceData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\RichInF1\referenceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{612F1D97-299F-451E-8170-DF18BF372856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8650D628-14F6-4F3B-B904-3B3917E6467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF1901F9-C066-45CD-B6D8-EF92789F909A}"/>
   </bookViews>
@@ -403,11 +403,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C527578D-A583-46CC-876B-066F596737BD}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>